<commit_message>
CHARMS -- Workflow and test case updates
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/RASScenario_Consent_Adult.xlsx
+++ b/src/test/java/CHARMS/resources/RASScenario_Consent_Adult.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muzipovay2/AquaProjects/CBIIT-Test-Automation/src/test/java/CHARMS/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7EAE57-4838-184F-A57D-8ADB939A80C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363A8A5B-DE69-5142-89EF-0D98F69975A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17600" xr2:uid="{54739BCC-024D-1B43-9BD3-233381306DEA}"/>
   </bookViews>
@@ -1273,7 +1273,7 @@
     <t>LAR 2 Name</t>
   </si>
   <si>
-    <t>Test</t>
+    <t>TestProgression</t>
   </si>
 </sst>
 </file>
@@ -1708,7 +1708,7 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
CHARMS - Adding FHQ Patient from NV
</commit_message>
<xml_diff>
--- a/src/test/java/CHARMS/resources/RASScenario_Consent_Adult.xlsx
+++ b/src/test/java/CHARMS/resources/RASScenario_Consent_Adult.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muzipovay2/AquaProjects/CBIIT-Test-Automation/src/test/java/CHARMS/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2381F784-2EA0-1E4C-A079-0894D65AD513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8810814-A801-174F-ABED-AA9444657D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17600" xr2:uid="{54739BCC-024D-1B43-9BD3-233381306DEA}"/>
   </bookViews>
@@ -1708,7 +1708,7 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>